<commit_message>
Sprint Backlog updated for Sprint 2
</commit_message>
<xml_diff>
--- a/doc/task06/Scrum_Team_White_V5.xlsx
+++ b/doc/task06/Scrum_Team_White_V5.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20730"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yann/Documents/BFH Informatik/4 FS 2019 Module/SoED/project GIT/ch.bfh.bti7081.s2019.white/doc/task06/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hrkun\MagentaCLOUD\Weiterbildung\BFH Informatik\4. Semester\Softwareengineering and Design\ch.bfh.bti7081.s2019.white\doc\task06\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E27C6CDD-6BAA-9B4C-A06F-22B7E905B77F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A04B627B-CD46-445B-B4C3-FDF875977C4A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="940" yWindow="460" windowWidth="24680" windowHeight="15540" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,12 +18,14 @@
     <sheet name="Sprint Backlog" sheetId="2" r:id="rId3"/>
     <sheet name="BurndownChart" sheetId="4" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Sprint Backlog'!$A$1:$L$30</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="135">
   <si>
     <t>ID</t>
   </si>
@@ -409,13 +411,43 @@
   </si>
   <si>
     <t>Repository erstellen: DB Anknüpfung</t>
+  </si>
+  <si>
+    <t>Refactoring MainView</t>
+  </si>
+  <si>
+    <t>Refactoring HomeView</t>
+  </si>
+  <si>
+    <t>Refactoring SettingsView</t>
+  </si>
+  <si>
+    <t>Refactoring MoodView</t>
+  </si>
+  <si>
+    <t>Refactoring CalendarView</t>
+  </si>
+  <si>
+    <t>Refactoring TipsView</t>
+  </si>
+  <si>
+    <t>HomeView == MoodView1</t>
+  </si>
+  <si>
+    <t>HomeView mit 2 Containern: MoodView1 Container mit Slider, CalenderEntry Container. HomeView Slider --&gt; MoodView 2. Mood-Button --&gt; Mood1 == HomeView ohne Calendar</t>
+  </si>
+  <si>
+    <t>Klassendiagramm bzgl. Persistenz updaten</t>
+  </si>
+  <si>
+    <t>Ursprüngliches gemeinsames ObserverInterface auflösen und viewspezifisches Interface definieren</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -431,15 +463,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -458,11 +483,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -473,11 +493,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -501,15 +520,8 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Schlecht" xfId="1" builtinId="27"/>
+  <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -818,13 +830,13 @@
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" customWidth="1"/>
-    <col min="2" max="2" width="18.5" customWidth="1"/>
+    <col min="1" max="1" width="15.36328125" customWidth="1"/>
+    <col min="2" max="2" width="18.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="3" customFormat="1" ht="19.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" s="3" customFormat="1" ht="19.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -832,7 +844,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -840,7 +852,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -848,7 +860,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -856,12 +868,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -869,7 +881,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -877,7 +889,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -904,19 +916,19 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.83203125" customWidth="1"/>
-    <col min="2" max="2" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.1640625" customWidth="1"/>
-    <col min="4" max="4" width="7.33203125" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" customWidth="1"/>
-    <col min="6" max="6" width="13.1640625" customWidth="1"/>
-    <col min="7" max="7" width="10.1640625" customWidth="1"/>
-    <col min="8" max="8" width="14.5" customWidth="1"/>
+    <col min="1" max="1" width="3.81640625" customWidth="1"/>
+    <col min="2" max="2" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.1796875" customWidth="1"/>
+    <col min="4" max="4" width="7.36328125" customWidth="1"/>
+    <col min="5" max="5" width="11.6328125" customWidth="1"/>
+    <col min="6" max="6" width="13.1796875" customWidth="1"/>
+    <col min="7" max="7" width="10.1796875" customWidth="1"/>
+    <col min="8" max="8" width="14.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" s="3" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -942,7 +954,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="1" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" s="1" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -968,7 +980,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -994,7 +1006,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1020,7 +1032,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1046,7 +1058,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1072,7 +1084,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1098,7 +1110,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="80" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1137,30 +1149,32 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:L23"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.83203125" style="8" customWidth="1"/>
-    <col min="2" max="2" width="6.1640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="22.33203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="39.1640625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="4.81640625" style="8" customWidth="1"/>
+    <col min="2" max="2" width="6.1796875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="22.36328125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="39.1796875" style="2" customWidth="1"/>
     <col min="5" max="5" width="19" style="2" customWidth="1"/>
-    <col min="6" max="6" width="10.33203125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="9.83203125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="8.33203125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="7.83203125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="9.1640625" style="2" customWidth="1"/>
-    <col min="11" max="11" width="7.1640625" style="2" customWidth="1"/>
-    <col min="12" max="12" width="15.1640625" style="2" customWidth="1"/>
-    <col min="13" max="16384" width="8.83203125" style="2"/>
+    <col min="6" max="6" width="10.36328125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="9.81640625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="8.36328125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="7.81640625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="9.1796875" style="2" customWidth="1"/>
+    <col min="11" max="11" width="7.1796875" style="2" customWidth="1"/>
+    <col min="12" max="12" width="15.1796875" style="2" customWidth="1"/>
+    <col min="13" max="16384" width="8.81640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="4" customFormat="1" ht="64" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" s="4" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1198,7 +1212,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A2" s="8">
         <v>1.1000000000000001</v>
       </c>
@@ -1233,7 +1247,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3" s="8">
         <v>1.2</v>
       </c>
@@ -1265,7 +1279,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
         <v>111</v>
       </c>
@@ -1291,7 +1305,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="64" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A5" s="8">
         <v>1.3</v>
       </c>
@@ -1329,7 +1343,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A6" s="8">
         <v>1.4</v>
       </c>
@@ -1348,7 +1362,7 @@
       <c r="F6" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="G6" s="10" t="s">
+      <c r="G6" s="1" t="s">
         <v>79</v>
       </c>
       <c r="H6" s="2" t="s">
@@ -1367,7 +1381,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A7" s="8">
         <v>1.5</v>
       </c>
@@ -1386,7 +1400,7 @@
       <c r="F7" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="G7" s="1" t="s">
         <v>80</v>
       </c>
       <c r="H7" s="2" t="s">
@@ -1405,7 +1419,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A8" s="8">
         <v>1.6</v>
       </c>
@@ -1424,7 +1438,7 @@
       <c r="F8" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="G8" s="10" t="s">
+      <c r="G8" s="1" t="s">
         <v>81</v>
       </c>
       <c r="H8" s="2" t="s">
@@ -1443,7 +1457,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A9" s="8" t="s">
         <v>115</v>
       </c>
@@ -1478,7 +1492,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="8" t="s">
         <v>118</v>
       </c>
@@ -1504,7 +1518,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A11" s="8">
         <v>1.7</v>
       </c>
@@ -1542,7 +1556,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A12" s="8">
         <v>1.8</v>
       </c>
@@ -1580,7 +1594,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A13" s="8">
         <v>1.9</v>
       </c>
@@ -1615,7 +1629,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A14" s="8" t="s">
         <v>97</v>
       </c>
@@ -1650,7 +1664,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A15" s="8" t="s">
         <v>76</v>
       </c>
@@ -1669,7 +1683,7 @@
       <c r="F15" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="G15" s="9" t="s">
+      <c r="G15" s="2" t="s">
         <v>79</v>
       </c>
       <c r="H15" s="2" t="s">
@@ -1688,7 +1702,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="64" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" ht="58" x14ac:dyDescent="0.35">
       <c r="A16" s="8" t="s">
         <v>83</v>
       </c>
@@ -1720,12 +1734,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17" s="8" t="s">
         <v>85</v>
       </c>
       <c r="B17" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>55</v>
@@ -1743,7 +1757,7 @@
         <v>99</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I17" s="2">
         <v>4</v>
@@ -1758,7 +1772,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18" s="8" t="s">
         <v>85</v>
       </c>
@@ -1781,7 +1795,7 @@
         <v>99</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I18" s="2">
         <v>4</v>
@@ -1790,7 +1804,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A19" s="8" t="s">
         <v>98</v>
       </c>
@@ -1810,16 +1824,16 @@
         <v>82</v>
       </c>
       <c r="H19" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I19" s="2">
         <v>6</v>
       </c>
-      <c r="I19" s="2">
-        <v>4</v>
-      </c>
       <c r="L19" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="64" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" ht="58" x14ac:dyDescent="0.35">
       <c r="A20" s="8" t="s">
         <v>100</v>
       </c>
@@ -1842,7 +1856,7 @@
         <v>78</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I20" s="2">
         <v>4</v>
@@ -1851,7 +1865,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A21" s="8" t="s">
         <v>103</v>
       </c>
@@ -1886,7 +1900,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A22" s="8" t="s">
         <v>107</v>
       </c>
@@ -1921,21 +1935,213 @@
         <v>102</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B23" s="2">
+        <v>2</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="I23" s="2">
-        <f>SUM(I2:I22)</f>
-        <v>73</v>
-      </c>
-      <c r="J23" s="2">
-        <f t="shared" ref="J23:K23" si="0">SUM(J2:J22)</f>
-        <v>47</v>
-      </c>
-      <c r="K23" s="2">
-        <f t="shared" si="0"/>
-        <v>59</v>
+        <v>2</v>
+      </c>
+      <c r="L23" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B24" s="2">
+        <v>2</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I24" s="2">
+        <v>2</v>
+      </c>
+      <c r="L24" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B25" s="2">
+        <v>2</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I25" s="2">
+        <v>2</v>
+      </c>
+      <c r="L25" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B26" s="2">
+        <v>2</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I26" s="2">
+        <v>2</v>
+      </c>
+      <c r="L26" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B27" s="2">
+        <v>2</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I27" s="2">
+        <v>2</v>
+      </c>
+      <c r="L27" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B28" s="2">
+        <v>2</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I28" s="2">
+        <v>2</v>
+      </c>
+      <c r="L28" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="B29" s="2">
+        <v>2</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I29" s="2">
+        <v>6</v>
+      </c>
+      <c r="L29" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B30" s="2">
+        <v>2</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I30" s="2">
+        <v>2</v>
+      </c>
+      <c r="L30" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:L30" xr:uid="{C2711728-F763-41C5-8F51-14446DF19FAB}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="2"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <extLst>
@@ -1954,14 +2160,14 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" customWidth="1"/>
-    <col min="4" max="4" width="14.33203125" customWidth="1"/>
+    <col min="2" max="2" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.6328125" customWidth="1"/>
+    <col min="4" max="4" width="14.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="5" customFormat="1" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" s="5" customFormat="1" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>16</v>
       </c>
@@ -1975,7 +2181,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1989,7 +2195,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2003,7 +2209,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2017,7 +2223,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>1</v>
       </c>
@@ -2031,7 +2237,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>1</v>
       </c>
@@ -2045,7 +2251,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
class diagram updated, Sprintlog updated
</commit_message>
<xml_diff>
--- a/doc/task06/Scrum_Team_White_V5.xlsx
+++ b/doc/task06/Scrum_Team_White_V5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hrkun\MagentaCLOUD\Weiterbildung\BFH Informatik\4. Semester\Softwareengineering and Design\ch.bfh.bti7081.s2019.white\doc\task06\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BD10A36-1D2F-48A6-93DA-2F62ACAF7DED}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76E490F1-6DAF-4520-B6D9-C9BB82464ADA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="940" yWindow="460" windowWidth="24680" windowHeight="15540" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1156,8 +1156,8 @@
   <dimension ref="A1:L30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L28" sqref="L28"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1772,7 +1772,7 @@
         <v>2</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>8</v>
+        <v>135</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.35">
@@ -2071,7 +2071,7 @@
         <v>1</v>
       </c>
       <c r="L27" s="2" t="s">
-        <v>8</v>
+        <v>135</v>
       </c>
     </row>
     <row r="28" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">

</xml_diff>